<commit_message>
Diccionario y base final
</commit_message>
<xml_diff>
--- a/05_presentations/Varaible_dictionary.xlsx
+++ b/05_presentations/Varaible_dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guibo\Desktop\Proyectos personales\Neighborhood Legalization\05_presentations\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Desktop\Proyectos personales\Neighborhood_Legalization\05_presentations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDAF11AA-CF1B-4A31-9468-50B4CD8B6255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712ED7CF-3089-42E3-B642-42FD460281F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="26136" xr2:uid="{B2FEE0EA-A6BE-43B3-9118-A82E76B07CAA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B2FEE0EA-A6BE-43B3-9118-A82E76B07CAA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Componente</t>
   </si>
@@ -299,13 +299,40 @@
   </si>
   <si>
     <t>Diccionario de variables</t>
+  </si>
+  <si>
+    <t>T1_LG08_distance_towards_treated</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Distancia (TI: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>time-invariant</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>) a unidades tratadas durante todo el periodo de tiempo. Las unidades tratadas tiene una distancia de cero.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -364,7 +391,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -386,6 +413,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,7 +444,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -435,6 +468,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -444,35 +498,26 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -794,29 +839,29 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.44140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="36.77734375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.109375" style="7" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="1" width="22.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="17.45">
+      <c r="A1" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-    </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+    </row>
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="13.9">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -833,207 +878,215 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-    </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="6"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11"/>
-      <c r="B6" s="6"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+    <row r="3" spans="1:5" s="1" customFormat="1">
+      <c r="A3" s="19"/>
+      <c r="B3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="1:5" s="1" customFormat="1">
+      <c r="A4" s="20"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1">
+      <c r="A5" s="20"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:5" s="1" customFormat="1">
+      <c r="A6" s="20"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1">
+      <c r="A7" s="21"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+    </row>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="22.5">
+      <c r="A8" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="16">
-        <v>2005</v>
-      </c>
-      <c r="E8" s="16">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="14" t="s">
+      <c r="D8" s="12">
+        <v>2005</v>
+      </c>
+      <c r="E8" s="12">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="33.75">
+      <c r="A9" s="19"/>
+      <c r="B9" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="16">
-        <v>2005</v>
-      </c>
-      <c r="E9" s="16">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="14" t="s">
+      <c r="D9" s="24">
+        <v>2005</v>
+      </c>
+      <c r="E9" s="24">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="22.5">
+      <c r="A10" s="19"/>
+      <c r="B10" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="16">
-        <v>2005</v>
-      </c>
-      <c r="E10" s="16">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A11" s="17"/>
-      <c r="B11" s="14" t="s">
+      <c r="D10" s="12">
+        <v>2005</v>
+      </c>
+      <c r="E10" s="12">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="33.75">
+      <c r="A11" s="19"/>
+      <c r="B11" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="16">
-        <v>2005</v>
-      </c>
-      <c r="E11" s="16">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.25">
-      <c r="A12" s="17"/>
-      <c r="B12" s="14" t="s">
+      <c r="D11" s="24">
+        <v>2005</v>
+      </c>
+      <c r="E11" s="24">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="1" customFormat="1" ht="45">
+      <c r="A12" s="19"/>
+      <c r="B12" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="16">
-        <v>2005</v>
-      </c>
-      <c r="E12" s="16">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="30.6" x14ac:dyDescent="0.25">
-      <c r="A13" s="17"/>
-      <c r="B13" s="14" t="s">
+      <c r="D12" s="12">
+        <v>2005</v>
+      </c>
+      <c r="E12" s="12">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="33.75">
+      <c r="A13" s="19"/>
+      <c r="B13" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="16">
-        <v>2005</v>
-      </c>
-      <c r="E13" s="16">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A14" s="17"/>
-      <c r="B14" s="14" t="s">
+      <c r="D13" s="24">
+        <v>2005</v>
+      </c>
+      <c r="E13" s="24">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="22.5">
+      <c r="A14" s="19"/>
+      <c r="B14" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="16">
-        <v>2005</v>
-      </c>
-      <c r="E14" s="16">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.25">
-      <c r="A15" s="18"/>
-      <c r="B15" s="19" t="s">
+      <c r="D14" s="12">
+        <v>2005</v>
+      </c>
+      <c r="E14" s="12">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="22.5">
+      <c r="A15" s="19"/>
+      <c r="B15" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="21">
-        <v>2005</v>
-      </c>
-      <c r="E15" s="21">
-        <v>2019</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="24">
+        <v>2005</v>
+      </c>
+      <c r="E15" s="24">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="1" customFormat="1" ht="22.5">
+      <c r="A16" s="25"/>
+      <c r="B16" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D16" s="15">
+        <v>2005</v>
+      </c>
+      <c r="E16" s="15">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="1" customFormat="1">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="7"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="1" customFormat="1" ht="13.9">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="7"/>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
+    <row r="19" spans="1:5" s="1" customFormat="1" ht="13.9">
+      <c r="A19" s="9"/>
       <c r="B19" s="6"/>
       <c r="C19" s="7"/>
       <c r="D19" s="5"/>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="12"/>
+    <row r="20" spans="1:5" s="1" customFormat="1" ht="13.9">
+      <c r="A20" s="9"/>
       <c r="B20" s="6"/>
       <c r="C20" s="7"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="12"/>
+    <row r="21" spans="1:5" s="1" customFormat="1" ht="13.9">
+      <c r="A21" s="9"/>
       <c r="B21" s="6"/>
       <c r="C21" s="7"/>
       <c r="D21" s="5"/>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="10" t="s">
+    <row r="22" spans="1:5" ht="33.75">
+      <c r="A22" s="17" t="s">
         <v>22</v>
       </c>
       <c r="B22" s="6" t="s">
@@ -1049,8 +1102,8 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="11"/>
+    <row r="23" spans="1:5" ht="33.75">
+      <c r="A23" s="18"/>
       <c r="B23" s="6" t="s">
         <v>6</v>
       </c>
@@ -1064,8 +1117,8 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A24" s="11"/>
+    <row r="24" spans="1:5" ht="22.5">
+      <c r="A24" s="18"/>
       <c r="B24" s="6" t="s">
         <v>7</v>
       </c>
@@ -1079,8 +1132,8 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
+    <row r="25" spans="1:5" ht="56.25">
+      <c r="A25" s="18"/>
       <c r="B25" s="6" t="s">
         <v>4</v>
       </c>
@@ -1094,8 +1147,8 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
+    <row r="26" spans="1:5" ht="33.75">
+      <c r="A26" s="17" t="s">
         <v>21</v>
       </c>
       <c r="B26" s="6" t="s">
@@ -1111,8 +1164,8 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="30.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="11"/>
+    <row r="27" spans="1:5" ht="33.75">
+      <c r="A27" s="18"/>
       <c r="B27" s="6" t="s">
         <v>14</v>
       </c>
@@ -1126,8 +1179,8 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A28" s="11"/>
+    <row r="28" spans="1:5" ht="33.75">
+      <c r="A28" s="18"/>
       <c r="B28" s="6" t="s">
         <v>15</v>
       </c>
@@ -1141,8 +1194,8 @@
         <v>2019</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="51" x14ac:dyDescent="0.3">
-      <c r="A29" s="11"/>
+    <row r="29" spans="1:5" ht="56.25">
+      <c r="A29" s="18"/>
       <c r="B29" s="6" t="s">
         <v>16</v>
       </c>
@@ -1162,7 +1215,7 @@
     <mergeCell ref="A22:A25"/>
     <mergeCell ref="A26:A29"/>
     <mergeCell ref="A3:A7"/>
-    <mergeCell ref="A8:A15"/>
+    <mergeCell ref="A8:A16"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>